<commit_message>
JNJANZ Local Assortment KPIs Development Setup
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ_SAND/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ_SAND/Data/KPI Exclusions Template.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -73,13 +73,34 @@
     <t xml:space="preserve">Value2</t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
+    <t xml:space="preserve">lsos_own_manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty; Irrelevant; General Empty</t>
   </si>
   <si>
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
-    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
+    <t xml:space="preserve">Out of Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eye_hand_level_sos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_level_assortment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linear_product_length_out_of_store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local_msl</t>
   </si>
 </sst>
 </file>
@@ -136,7 +157,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,12 +176,6 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC99FF"/>
-        <bgColor rgb="FF9999FF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -209,15 +224,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,23 +313,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="208.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -324,15 +338,15 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -341,6 +355,57 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
JNJANZ Local Assortment KPIs : Code adjustments according to the new Assortment Template
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ_SAND/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ_SAND/Data/KPI Exclusions Template.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">linear_product_length_out_of_store</t>
   </si>
   <si>
-    <t xml:space="preserve">local_msl</t>
+    <t xml:space="preserve">Distribution</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,6 +140,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -211,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +240,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -321,10 +331,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.165991902834"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -401,7 +411,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="4"/>

</xml_diff>